<commit_message>
Divided scripts for all figures. For TiTv figure we added the difference between adults and pediatric cases and also the purest Relapse matched code
</commit_message>
<xml_diff>
--- a/MEAndCooccurence.xlsx
+++ b/MEAndCooccurence.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/Projects/Statistics WGS paper/WGS_Statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90CEDD7-AF85-1648-AB1F-D33A0AF9E8F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="5320" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pediatric" sheetId="1" r:id="rId1"/>
     <sheet name="Adults" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -396,7 +397,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -449,6 +450,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -716,14 +720,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -735,179 +742,187 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -917,11 +932,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,7 +1071,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>88</v>
@@ -1064,7 +1079,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>89</v>
@@ -1072,7 +1087,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>90</v>
@@ -1080,7 +1095,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>91</v>
@@ -1088,7 +1103,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>92</v>
@@ -1096,7 +1111,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>93</v>
@@ -1104,7 +1119,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>94</v>
@@ -1112,7 +1127,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>95</v>
@@ -1120,7 +1135,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>96</v>
@@ -1128,7 +1143,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>97</v>
@@ -1136,7 +1151,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>98</v>
@@ -1144,7 +1159,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>99</v>
@@ -1152,109 +1167,105 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="B45" s="1"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
@@ -1271,10 +1282,6 @@
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>